<commit_message>
Import data from Excel to SL Server button
</commit_message>
<xml_diff>
--- a/MyShopDataImportDataBase.xlsx
+++ b/MyShopDataImportDataBase.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\21810012_MyShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1176,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,7 +1219,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>17</v>
@@ -1242,7 +1242,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>13</v>
@@ -1265,7 +1265,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>15</v>
@@ -1288,7 +1288,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>18</v>
@@ -1311,7 +1311,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>19</v>
@@ -1334,7 +1334,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>20</v>
@@ -1357,7 +1357,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>22</v>
@@ -1380,7 +1380,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>24</v>
@@ -1403,7 +1403,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>26</v>
@@ -1426,7 +1426,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>28</v>
@@ -1449,7 +1449,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>30</v>
@@ -1472,7 +1472,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>32</v>
@@ -1495,7 +1495,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>34</v>
@@ -1518,7 +1518,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>36</v>
@@ -1541,7 +1541,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>37</v>
@@ -1564,7 +1564,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>38</v>
@@ -1587,7 +1587,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>39</v>
@@ -1610,7 +1610,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>40</v>
@@ -1633,7 +1633,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>41</v>
@@ -1656,7 +1656,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>42</v>
@@ -1679,7 +1679,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>44</v>
@@ -1702,7 +1702,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>46</v>
@@ -1725,7 +1725,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>48</v>
@@ -1748,7 +1748,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>50</v>
@@ -1771,7 +1771,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>52</v>
@@ -1794,7 +1794,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>54</v>
@@ -1817,7 +1817,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>56</v>
@@ -1840,7 +1840,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>58</v>
@@ -1863,7 +1863,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>60</v>
@@ -1886,7 +1886,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>62</v>
@@ -1909,7 +1909,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>64</v>
@@ -1932,7 +1932,7 @@
         <v>32</v>
       </c>
       <c r="C34" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>66</v>
@@ -1955,7 +1955,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>68</v>
@@ -1978,7 +1978,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>70</v>
@@ -2001,7 +2001,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>72</v>
@@ -2024,7 +2024,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>74</v>
@@ -2047,7 +2047,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>76</v>
@@ -2070,7 +2070,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>78</v>
@@ -2093,7 +2093,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>80</v>
@@ -2116,7 +2116,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>82</v>
@@ -2139,7 +2139,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>84</v>
@@ -2162,7 +2162,7 @@
         <v>42</v>
       </c>
       <c r="C44" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>86</v>
@@ -2185,7 +2185,7 @@
         <v>43</v>
       </c>
       <c r="C45" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>87</v>
@@ -2208,7 +2208,7 @@
         <v>44</v>
       </c>
       <c r="C46" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>89</v>
@@ -2231,7 +2231,7 @@
         <v>45</v>
       </c>
       <c r="C47" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>90</v>
@@ -2254,7 +2254,7 @@
         <v>46</v>
       </c>
       <c r="C48" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>92</v>
@@ -2277,7 +2277,7 @@
         <v>47</v>
       </c>
       <c r="C49" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>94</v>
@@ -2300,7 +2300,7 @@
         <v>48</v>
       </c>
       <c r="C50" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>96</v>
@@ -2323,7 +2323,7 @@
         <v>49</v>
       </c>
       <c r="C51" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>98</v>
@@ -2346,7 +2346,7 @@
         <v>50</v>
       </c>
       <c r="C52" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>100</v>
@@ -2369,7 +2369,7 @@
         <v>51</v>
       </c>
       <c r="C53" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>103</v>
@@ -2392,7 +2392,7 @@
         <v>52</v>
       </c>
       <c r="C54" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>104</v>
@@ -2415,7 +2415,7 @@
         <v>53</v>
       </c>
       <c r="C55" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>106</v>
@@ -2438,7 +2438,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>108</v>
@@ -2461,7 +2461,7 @@
         <v>55</v>
       </c>
       <c r="C57" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>110</v>
@@ -2484,7 +2484,7 @@
         <v>56</v>
       </c>
       <c r="C58" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>112</v>
@@ -2507,7 +2507,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>114</v>
@@ -2530,7 +2530,7 @@
         <v>58</v>
       </c>
       <c r="C60" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>116</v>
@@ -2553,7 +2553,7 @@
         <v>59</v>
       </c>
       <c r="C61" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>118</v>
@@ -2576,7 +2576,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
Added Sach Window CRUD, row per page, search name, filter price, view detail functions
</commit_message>
<xml_diff>
--- a/MyShopDataImportDataBase.xlsx
+++ b/MyShopDataImportDataBase.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="228">
   <si>
     <t>ID</t>
   </si>
@@ -516,186 +516,6 @@
     <t>sale2</t>
   </si>
   <si>
-    <t>Images/Sach/TinhCam/tinhCam01.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TinhCam/tinhCam02.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TinhCam/tinhCam03.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TinhCam/tinhCam04.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TinhCam/tinhCam05.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TinhCam/tinhCam06.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TinhCam/tinhCam07.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TinhCam/tinhCam08.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TinhCam/tinhCam09.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TinhCam/tinhCam10.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TinhCam/tinhCam11.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TinhCam/tinhCam12.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/GiaTuongVaKhoaHocVienTuong/khoaHocVienTuong01.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/GiaTuongVaKhoaHocVienTuong/khoaHocVienTuong02.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/GiaTuongVaKhoaHocVienTuong/khoaHocVienTuong03.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/GiaTuongVaKhoaHocVienTuong/khoaHocVienTuong04.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/GiaTuongVaKhoaHocVienTuong/khoaHocVienTuong05.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/GiaTuongVaKhoaHocVienTuong/khoaHocVienTuong06.jpeg</t>
-  </si>
-  <si>
-    <t>Images/Sach/GiaTuongVaKhoaHocVienTuong/khoaHocVienTuong07.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/GiaTuongVaKhoaHocVienTuong/khoaHocVienTuong08.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/GiaTuongVaKhoaHocVienTuong/khoaHocVienTuong09.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/GiaTuongVaKhoaHocVienTuong/khoaHocVienTuong10.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/GiaTuongVaKhoaHocVienTuong/khoaHocVienTuong11.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/GiaTuongVaKhoaHocVienTuong/khoaHocVienTuong12.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenCamHung/truyenCamHung01.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenCamHung/truyenCamHung02.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenCamHung/truyenCamHung03.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenCamHung/truyenCamHung04.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenCamHung/truyenCamHung05.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenCamHung/truyenCamHung06.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenCamHung/truyenCamHung07.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenCamHung/truyenCamHung08.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenCamHung/truyenCamHung09.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenCamHung/truyenCamHung10.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenCamHung/truyenCamHung11.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenCamHung/truyenCamHung12.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenNgan/truyenNgan01.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenNgan/truyenNgan02.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenNgan/truyenNgan03.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenNgan/truyenNgan04.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenNgan/truyenNgan05.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenNgan/truyenNgan06.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenNgan/truyenNgan07.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenNgan/truyenNgan08.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenNgan/truyenNgan09.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenNgan/truyenNgan10.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenNgan/truyenNgan11.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/TruyenNgan/truyenNgan12.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/DayNauAn/dayNauAn01.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/DayNauAn/dayNauAn02.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/DayNauAn/dayNauAn03.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/DayNauAn/dayNauAn04.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/DayNauAn/dayNauAn05.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/DayNauAn/dayNauAn06.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/DayNauAn/dayNauAn07.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/DayNauAn/dayNauAn08.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/DayNauAn/dayNauAn09.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/DayNauAn/dayNauAn10.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/DayNauAn/dayNauAn11.jpg</t>
-  </si>
-  <si>
-    <t>Images/Sach/DayNauAn/dayNauAn12.jpg</t>
-  </si>
-  <si>
     <t>Images/KhachHang/avatar_01.jpg</t>
   </si>
   <si>
@@ -709,6 +529,189 @@
   </si>
   <si>
     <t>Images/KhachHang/avatar_05.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_01.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_02.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_03.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_04.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_05.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_06.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_07.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_08.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_09.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_10.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_11.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_12.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_13.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_14.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_15.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_16.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_17.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_19.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_20.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_21.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_22.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_23.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_24.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_25.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_26.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_27.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_28.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_29.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_30.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_31.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_32.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_33.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_34.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_35.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_36.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_37.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_38.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_39.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_40.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_41.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_42.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_43.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_44.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_45.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_46.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_47.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_48.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_49.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_50.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_51.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_52.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_53.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_54.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_55.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_56.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_57.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_58.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_59.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_60.jpg</t>
+  </si>
+  <si>
+    <t>Images/Sach/sach_18.jpeg</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -760,7 +763,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -779,8 +782,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -803,12 +812,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -825,6 +845,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1106,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C7"/>
+  <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,42 +1151,50 @@
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3" t="s">
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3" t="s">
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1174,10 +1206,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H62"/>
+  <dimension ref="B2:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,9 +1221,10 @@
     <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="31.5703125" customWidth="1"/>
     <col min="8" max="8" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1214,12 +1247,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>17</v>
@@ -1234,15 +1267,18 @@
         <v>12</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>13</v>
@@ -1257,15 +1293,15 @@
         <v>14</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>3</v>
       </c>
       <c r="C5" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>15</v>
@@ -1280,15 +1316,15 @@
         <v>14</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>4</v>
       </c>
       <c r="C6" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>18</v>
@@ -1303,15 +1339,15 @@
         <v>14</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>5</v>
       </c>
       <c r="C7" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>19</v>
@@ -1326,15 +1362,15 @@
         <v>16</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>6</v>
       </c>
       <c r="C8" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>20</v>
@@ -1349,15 +1385,15 @@
         <v>21</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>7</v>
       </c>
       <c r="C9" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>22</v>
@@ -1372,15 +1408,15 @@
         <v>23</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>8</v>
       </c>
       <c r="C10" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>24</v>
@@ -1395,15 +1431,15 @@
         <v>25</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>9</v>
       </c>
       <c r="C11" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>26</v>
@@ -1418,15 +1454,15 @@
         <v>27</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>10</v>
       </c>
       <c r="C12" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>28</v>
@@ -1441,15 +1477,15 @@
         <v>29</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>11</v>
       </c>
       <c r="C13" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>30</v>
@@ -1464,15 +1500,15 @@
         <v>31</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>12</v>
       </c>
       <c r="C14" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>32</v>
@@ -1487,15 +1523,15 @@
         <v>33</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
         <v>13</v>
       </c>
       <c r="C15" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>34</v>
@@ -1509,16 +1545,16 @@
       <c r="G15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
         <v>14</v>
       </c>
       <c r="C16" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>36</v>
@@ -1532,8 +1568,8 @@
       <c r="G16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>175</v>
+      <c r="H16" s="5" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1541,7 +1577,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>37</v>
@@ -1555,8 +1591,8 @@
       <c r="G17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>176</v>
+      <c r="H17" s="5" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1564,7 +1600,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>38</v>
@@ -1578,8 +1614,8 @@
       <c r="G18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>177</v>
+      <c r="H18" s="5" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1587,7 +1623,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>39</v>
@@ -1601,8 +1637,8 @@
       <c r="G19" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="6" t="s">
-        <v>178</v>
+      <c r="H19" s="5" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1610,7 +1646,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>40</v>
@@ -1624,8 +1660,8 @@
       <c r="G20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>179</v>
+      <c r="H20" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1633,7 +1669,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>41</v>
@@ -1647,8 +1683,8 @@
       <c r="G21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>180</v>
+      <c r="H21" s="5" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1656,7 +1692,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>42</v>
@@ -1670,8 +1706,8 @@
       <c r="G22" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>181</v>
+      <c r="H22" s="5" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1679,7 +1715,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>44</v>
@@ -1693,8 +1729,8 @@
       <c r="G23" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="6" t="s">
-        <v>182</v>
+      <c r="H23" s="5" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1702,7 +1738,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>46</v>
@@ -1716,8 +1752,8 @@
       <c r="G24" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>183</v>
+      <c r="H24" s="5" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1725,7 +1761,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>48</v>
@@ -1739,8 +1775,8 @@
       <c r="G25" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>184</v>
+      <c r="H25" s="5" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1748,7 +1784,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>50</v>
@@ -1762,8 +1798,8 @@
       <c r="G26" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H26" s="6" t="s">
-        <v>185</v>
+      <c r="H26" s="5" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1771,7 +1807,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>52</v>
@@ -1785,8 +1821,8 @@
       <c r="G27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>186</v>
+      <c r="H27" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -1794,7 +1830,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>54</v>
@@ -1808,8 +1844,8 @@
       <c r="G28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>187</v>
+      <c r="H28" s="5" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -1817,7 +1853,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>56</v>
@@ -1831,8 +1867,8 @@
       <c r="G29" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>188</v>
+      <c r="H29" s="5" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -1840,7 +1876,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>58</v>
@@ -1854,8 +1890,8 @@
       <c r="G30" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H30" s="6" t="s">
-        <v>189</v>
+      <c r="H30" s="5" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -1863,7 +1899,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>60</v>
@@ -1877,8 +1913,8 @@
       <c r="G31" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>190</v>
+      <c r="H31" s="5" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -1886,7 +1922,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>62</v>
@@ -1900,8 +1936,8 @@
       <c r="G32" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>191</v>
+      <c r="H32" s="5" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -1909,7 +1945,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>64</v>
@@ -1923,8 +1959,8 @@
       <c r="G33" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H33" s="6" t="s">
-        <v>192</v>
+      <c r="H33" s="5" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -1932,7 +1968,7 @@
         <v>32</v>
       </c>
       <c r="C34" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>66</v>
@@ -1946,8 +1982,8 @@
       <c r="G34" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>193</v>
+      <c r="H34" s="5" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -1955,7 +1991,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>68</v>
@@ -1969,8 +2005,8 @@
       <c r="G35" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>194</v>
+      <c r="H35" s="5" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -1978,7 +2014,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>70</v>
@@ -1992,8 +2028,8 @@
       <c r="G36" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="H36" s="6" t="s">
-        <v>195</v>
+      <c r="H36" s="5" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -2001,7 +2037,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>72</v>
@@ -2015,8 +2051,8 @@
       <c r="G37" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="H37" s="6" t="s">
-        <v>196</v>
+      <c r="H37" s="5" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -2024,7 +2060,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>74</v>
@@ -2038,8 +2074,8 @@
       <c r="G38" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="H38" s="6" t="s">
-        <v>197</v>
+      <c r="H38" s="5" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
@@ -2047,7 +2083,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>76</v>
@@ -2061,8 +2097,8 @@
       <c r="G39" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="H39" s="6" t="s">
-        <v>198</v>
+      <c r="H39" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
@@ -2070,7 +2106,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>78</v>
@@ -2084,8 +2120,8 @@
       <c r="G40" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="H40" s="6" t="s">
-        <v>199</v>
+      <c r="H40" s="5" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
@@ -2093,7 +2129,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>80</v>
@@ -2107,8 +2143,8 @@
       <c r="G41" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H41" s="6" t="s">
-        <v>200</v>
+      <c r="H41" s="5" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -2116,7 +2152,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>82</v>
@@ -2130,8 +2166,8 @@
       <c r="G42" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H42" s="6" t="s">
-        <v>201</v>
+      <c r="H42" s="5" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -2139,7 +2175,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>84</v>
@@ -2153,8 +2189,8 @@
       <c r="G43" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H43" s="6" t="s">
-        <v>202</v>
+      <c r="H43" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
@@ -2162,7 +2198,7 @@
         <v>42</v>
       </c>
       <c r="C44" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>86</v>
@@ -2176,8 +2212,8 @@
       <c r="G44" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H44" s="6" t="s">
-        <v>203</v>
+      <c r="H44" s="5" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
@@ -2185,7 +2221,7 @@
         <v>43</v>
       </c>
       <c r="C45" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>87</v>
@@ -2199,8 +2235,8 @@
       <c r="G45" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="H45" s="6" t="s">
-        <v>204</v>
+      <c r="H45" s="5" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
@@ -2208,7 +2244,7 @@
         <v>44</v>
       </c>
       <c r="C46" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>89</v>
@@ -2222,8 +2258,8 @@
       <c r="G46" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H46" s="6" t="s">
-        <v>205</v>
+      <c r="H46" s="5" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
@@ -2231,7 +2267,7 @@
         <v>45</v>
       </c>
       <c r="C47" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>90</v>
@@ -2245,8 +2281,8 @@
       <c r="G47" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H47" s="6" t="s">
-        <v>206</v>
+      <c r="H47" s="5" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -2254,7 +2290,7 @@
         <v>46</v>
       </c>
       <c r="C48" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>92</v>
@@ -2268,8 +2304,8 @@
       <c r="G48" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H48" s="6" t="s">
-        <v>207</v>
+      <c r="H48" s="5" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -2277,7 +2313,7 @@
         <v>47</v>
       </c>
       <c r="C49" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>94</v>
@@ -2291,8 +2327,8 @@
       <c r="G49" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="H49" s="6" t="s">
-        <v>208</v>
+      <c r="H49" s="5" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
@@ -2300,7 +2336,7 @@
         <v>48</v>
       </c>
       <c r="C50" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>96</v>
@@ -2314,8 +2350,8 @@
       <c r="G50" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="H50" s="6" t="s">
-        <v>209</v>
+      <c r="H50" s="5" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
@@ -2323,7 +2359,7 @@
         <v>49</v>
       </c>
       <c r="C51" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>98</v>
@@ -2337,8 +2373,8 @@
       <c r="G51" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="H51" s="6" t="s">
-        <v>210</v>
+      <c r="H51" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
@@ -2346,7 +2382,7 @@
         <v>50</v>
       </c>
       <c r="C52" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>100</v>
@@ -2360,8 +2396,8 @@
       <c r="G52" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H52" s="6" t="s">
-        <v>211</v>
+      <c r="H52" s="5" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
@@ -2369,7 +2405,7 @@
         <v>51</v>
       </c>
       <c r="C53" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>103</v>
@@ -2383,8 +2419,8 @@
       <c r="G53" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="H53" s="6" t="s">
-        <v>212</v>
+      <c r="H53" s="5" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
@@ -2392,7 +2428,7 @@
         <v>52</v>
       </c>
       <c r="C54" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>104</v>
@@ -2406,8 +2442,8 @@
       <c r="G54" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H54" s="6" t="s">
-        <v>213</v>
+      <c r="H54" s="5" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
@@ -2415,7 +2451,7 @@
         <v>53</v>
       </c>
       <c r="C55" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>106</v>
@@ -2429,8 +2465,8 @@
       <c r="G55" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H55" s="7" t="s">
-        <v>214</v>
+      <c r="H55" s="5" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
@@ -2438,7 +2474,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>108</v>
@@ -2452,8 +2488,8 @@
       <c r="G56" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="H56" s="6" t="s">
-        <v>215</v>
+      <c r="H56" s="5" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
@@ -2461,7 +2497,7 @@
         <v>55</v>
       </c>
       <c r="C57" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>110</v>
@@ -2475,8 +2511,8 @@
       <c r="G57" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="H57" s="6" t="s">
-        <v>216</v>
+      <c r="H57" s="5" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
@@ -2484,7 +2520,7 @@
         <v>56</v>
       </c>
       <c r="C58" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>112</v>
@@ -2498,8 +2534,8 @@
       <c r="G58" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="H58" s="6" t="s">
-        <v>217</v>
+      <c r="H58" s="5" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
@@ -2507,7 +2543,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>114</v>
@@ -2521,8 +2557,8 @@
       <c r="G59" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="H59" s="7" t="s">
-        <v>218</v>
+      <c r="H59" s="5" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -2530,7 +2566,7 @@
         <v>58</v>
       </c>
       <c r="C60" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>116</v>
@@ -2544,8 +2580,8 @@
       <c r="G60" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="H60" s="6" t="s">
-        <v>219</v>
+      <c r="H60" s="5" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -2553,7 +2589,7 @@
         <v>59</v>
       </c>
       <c r="C61" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>118</v>
@@ -2567,8 +2603,8 @@
       <c r="G61" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H61" s="6" t="s">
-        <v>220</v>
+      <c r="H61" s="5" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
@@ -2576,7 +2612,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>120</v>
@@ -2590,8 +2626,8 @@
       <c r="G62" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="H62" s="6" t="s">
-        <v>221</v>
+      <c r="H62" s="5" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2654,7 +2690,7 @@
         <v>127</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>222</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -2674,7 +2710,7 @@
         <v>130</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>223</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -2694,7 +2730,7 @@
         <v>133</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>224</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -2714,7 +2750,7 @@
         <v>136</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>225</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -2734,7 +2770,7 @@
         <v>149</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>226</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>